<commit_message>
test to get cell color
</commit_message>
<xml_diff>
--- a/3-Dev/DevApp/Files/CellFormats.xlsx
+++ b/3-Dev/DevApp/Files/CellFormats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a990f455bb745add/ProjetsDev/10-Pierlam/OpenExcelSdk/Dev/OpenExcelSdk/3-Dev/DevApp/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_AD4DB114E441178AC67DF4536695FF58683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AFF0D35-7441-4191-9A40-5743ACAB4BE1}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_AD4DB114E441178AC67DF4536695FF58683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE212BE8-7A8E-4E2B-9F47-B20B67BF031A}"/>
   <bookViews>
-    <workbookView xWindow="11910" yWindow="3000" windowWidth="16260" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6960" yWindow="3030" windowWidth="16155" windowHeight="8520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>value</t>
   </si>
   <si>
     <t>info</t>
+  </si>
+  <si>
+    <t>int, border</t>
+  </si>
+  <si>
+    <t>int, bgcolor</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>theme</t>
   </si>
 </sst>
 </file>
@@ -46,7 +58,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -59,8 +71,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -68,13 +98,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -90,6 +139,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -355,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -367,12 +420,44 @@
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="5">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add ExportStyles of an excel to an output excel + GetCellColor
</commit_message>
<xml_diff>
--- a/3-Dev/DevApp/Files/CellFormats.xlsx
+++ b/3-Dev/DevApp/Files/CellFormats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a990f455bb745add/ProjetsDev/10-Pierlam/OpenExcelSdk/Dev/OpenExcelSdk/3-Dev/DevApp/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_AD4DB114E441178AC67DF4536695FF58683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE212BE8-7A8E-4E2B-9F47-B20B67BF031A}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_AD4DB114E441178AC67DF4536695FF58683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBB4E1CF-DAFC-4DE0-9C52-D7AA8F6AC1BA}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="3030" windowWidth="16155" windowHeight="8520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>value</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>theme</t>
+  </si>
+  <si>
+    <t>with gradient</t>
   </si>
 </sst>
 </file>
@@ -58,7 +61,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,6 +89,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE4FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -117,19 +126,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFE4FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -139,10 +155,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +472,30 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>46001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>